<commit_message>
refactoring to not need batching
</commit_message>
<xml_diff>
--- a/armonk_results.xlsx
+++ b/armonk_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nfberthusen\Documents\Projects\Research\benewop-benchmarking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FBE9A7F-0FBF-43CD-87F2-EFA21C39E020}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A584D97D-F747-4930-AAF9-2139B1808841}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="16" xr2:uid="{A83D9AE7-01C1-4705-9240-4A7C990C7FB0}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" firstSheet="3" activeTab="19" xr2:uid="{A83D9AE7-01C1-4705-9240-4A7C990C7FB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Armonk0" sheetId="3" r:id="rId1"/>
@@ -30,9 +30,11 @@
     <sheet name="Jojo13" sheetId="18" r:id="rId15"/>
     <sheet name="Jojo14" sheetId="19" r:id="rId16"/>
     <sheet name="Jojo15" sheetId="20" r:id="rId17"/>
+    <sheet name="Jojo16" sheetId="21" r:id="rId18"/>
+    <sheet name="Jojo17" sheetId="22" r:id="rId19"/>
+    <sheet name="Jojo18" sheetId="23" r:id="rId20"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -50,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="761">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1297" uniqueCount="867">
   <si>
     <t>Sigma = 336</t>
   </si>
@@ -2333,6 +2335,324 @@
   </si>
   <si>
     <t>Conversion constant: 15.113382279092622. Exponent: -0.9420720154939807</t>
+  </si>
+  <si>
+    <t>Pi Amplitude = 0.9255702985634208</t>
+  </si>
+  <si>
+    <t>Pi Amplitude = 0.9002837456502224</t>
+  </si>
+  <si>
+    <t>Pi Amplitude = 0.8125224123005497</t>
+  </si>
+  <si>
+    <t>Pi Amplitude = 0.54164904240245</t>
+  </si>
+  <si>
+    <t>Pi Amplitude = 0.18186309701223674</t>
+  </si>
+  <si>
+    <t>Pi Amplitude = 0.12702749286796988</t>
+  </si>
+  <si>
+    <t>Pi Amplitude = 0.08046901719369828</t>
+  </si>
+  <si>
+    <t>['5efa3367f3a1b300132cd0f7',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa33691f31490012fddb76',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa336c20eee10013be430c',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa336e04f6d40013665bca',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa337004f6d40013665bcb',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa337311d14f0013abecf3',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa337620eee10013be430d',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa337920eee10013be430f']</t>
+  </si>
+  <si>
+    <t>[[16, 80, 0.9255702985634208],</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [16, 112, 0.9002837456502224],</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [16, 176, 0.8125224123005497],</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [32, 256, 0.54164904240245],</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [80, 608, 0.18186309701223674],</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [112, 944, 0.12702749286796988],</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [176, 1440, 0.08046901719369828]]</t>
+  </si>
+  <si>
+    <t>Pi Amplitude = 0.3702369874891184</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [48, 400, 0.3702369874891184],</t>
+  </si>
+  <si>
+    <t>Period = 87.74328452860695</t>
+  </si>
+  <si>
+    <t>Period = 197.85084515365193</t>
+  </si>
+  <si>
+    <t>Period = 388.3027063078206</t>
+  </si>
+  <si>
+    <t>Period = 547.3716399870816</t>
+  </si>
+  <si>
+    <t>Period = 861.1932667605826</t>
+  </si>
+  <si>
+    <t>['5efa40fb1c6a20001272eb0a',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa40fe2aeb6200123d2be1',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa4101f3a1b300132cd1fd',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa41031f31490012fddc55',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa4106f3a1b300132cd1fe',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa41091f31490012fddc56',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa410d2aeb6200123d2be3',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa411120eee10013be43ee']</t>
+  </si>
+  <si>
+    <t>Period = 138.82800013054782</t>
+  </si>
+  <si>
+    <t>Period = 95.94887545086506</t>
+  </si>
+  <si>
+    <t>Period = 85.60944330663746</t>
+  </si>
+  <si>
+    <t>Conversion constant: 76.16056132506117. Exponent: -0.9607519043146192</t>
+  </si>
+  <si>
+    <t>Conversion constant: 16.434457262102157. Exponent: -0.9389201013042705</t>
+  </si>
+  <si>
+    <t>Pi Amplitude = 0.8694900512886118</t>
+  </si>
+  <si>
+    <t>Pi Amplitude = 0.8674870203693015</t>
+  </si>
+  <si>
+    <t>Pi Amplitude = 0.8039648763939761</t>
+  </si>
+  <si>
+    <t>Pi Amplitude = 0.4256695203330245</t>
+  </si>
+  <si>
+    <t>Pi Amplitude = 0.2728874688691777</t>
+  </si>
+  <si>
+    <t>Pi Amplitude = 0.160775094300207</t>
+  </si>
+  <si>
+    <t>Pi Amplitude = 0.11266391095916693</t>
+  </si>
+  <si>
+    <t>Pi Amplitude = 0.0706996391426449</t>
+  </si>
+  <si>
+    <t>['5efa4c291c6a20001272ebb8',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa4c2b2aeb6200123d2c69',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa4c2d04f6d40013665d48',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa4c2f6920cd00125239e9',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa4c317c0d6800137ffda4',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa4c341c6a20001272ebb9',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa4c372aeb6200123d2c6b',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa4c3a6920cd00125239ea']</t>
+  </si>
+  <si>
+    <t>[[16, 80, 0.8694900512886118],</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [16, 112, 0.8674870203693015],</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [16, 176, 0.8039648763939761],</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [32, 256, 0.4256695203330245],</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [48, 400, 0.2728874688691777],</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [80, 608, 0.160775094300207],</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [112, 944, 0.11266391095916693],</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [176, 1440, 0.0706996391426449]]</t>
+  </si>
+  <si>
+    <t>Period = 154.18822787816336</t>
+  </si>
+  <si>
+    <t>Period = 233.3159998399876</t>
+  </si>
+  <si>
+    <t>Period = 383.9691696084671</t>
+  </si>
+  <si>
+    <t>Period = 535.0791573074756</t>
+  </si>
+  <si>
+    <t>Period = 857.2840535651976</t>
+  </si>
+  <si>
+    <t>['5efa57ed2aeb6200123d2d9c',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa57f01f31490012fdde08',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa57f32aeb6200123d2d9d',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa57f61c6a20001272ece3',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa57f96920cd0012523b0e',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa57fc03510e00123c9b2e',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa580004f6d40013665e81',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa580403510e00123c9b31']</t>
+  </si>
+  <si>
+    <t>Period = 80.05953915145214</t>
+  </si>
+  <si>
+    <t>Period = 79.94524312025808</t>
+  </si>
+  <si>
+    <t>Period = 85.57704236605974</t>
+  </si>
+  <si>
+    <t>Conversion constant: 66.61375917115514. Exponent: -0.9620204924453801</t>
+  </si>
+  <si>
+    <t>Conversion constant: 13.78818074531042. Exponent: -0.9609761215025634</t>
+  </si>
+  <si>
+    <t>Pi Amplitude = 1.0005842657491106</t>
+  </si>
+  <si>
+    <t>Pi Amplitude = 1.1187475076579876</t>
+  </si>
+  <si>
+    <t>Pi Amplitude = 1.4502576316771583</t>
+  </si>
+  <si>
+    <t>Pi Amplitude = 0.5167989756559059</t>
+  </si>
+  <si>
+    <t>Pi Amplitude = 0.33947366820624686</t>
+  </si>
+  <si>
+    <t>Pi Amplitude = 0.1969268097967586</t>
+  </si>
+  <si>
+    <t>Pi Amplitude = 0.1412534989707599</t>
+  </si>
+  <si>
+    <t>Pi Amplitude = 0.09029120594590444</t>
+  </si>
+  <si>
+    <t>['5efa6bd26920cd0012523c07',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa6bd520eee10013be46be',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa6bd720eee10013be46c0',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa6bd803510e00123c9c5a',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa6bdbf3a1b300132cd50a',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa6bdd6920cd0012523c09',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa6be003510e00123c9c5c',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> '5efa6be320eee10013be46c3']</t>
+  </si>
+  <si>
+    <t>[[16, 80, 1.000],</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [32, 256, 0.5167989756559059],</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [48, 400, 0.33947366820624686],</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [80, 608, 0.1969268097967586],</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [112, 944, 0.1412534989707599],</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [176, 1440, 0.09029120594590444]]</t>
   </si>
 </sst>
 </file>
@@ -3477,6 +3797,260 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="7680960" y="5486400"/>
+          <a:ext cx="4107180" cy="2667000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing18.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>102870</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F0BC997-ECD2-4C22-98E5-191E3E59D064}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7680960" y="2194560"/>
+          <a:ext cx="3943350" cy="2667000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3065A6BF-96B6-44D4-896C-B4852F2BEE7D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7680960" y="5303520"/>
+          <a:ext cx="4107180" cy="2667000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing19.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>102870</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7B3F148-743C-4ECF-B29E-FDAAD85B2879}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7680960" y="1828800"/>
+          <a:ext cx="3943350" cy="2667000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{165045D2-CFCE-4C5F-8D6C-1DC4B9FC4D20}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7680960" y="4937760"/>
           <a:ext cx="4107180" cy="2667000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7828,7 +8402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEE54EEC-C847-411B-B72C-A066C3BD4F4A}">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
@@ -8108,6 +8682,591 @@
     <row r="46" spans="13:13">
       <c r="M46" s="1" t="s">
         <v>760</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15945C47-5CCD-43CD-A427-F537D2A253E6}">
+  <dimension ref="A1:M45"/>
+  <sheetViews>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="M45" sqref="M45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="M3" s="1" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="2"/>
+      <c r="E4" s="1" t="s">
+        <v>771</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="M6" s="1" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="2"/>
+      <c r="E8" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="2"/>
+      <c r="E12" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>779</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="2"/>
+      <c r="E16" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="2"/>
+      <c r="I20" s="1" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="2"/>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="1" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" s="2"/>
+      <c r="M28" s="1" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" s="1" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="45" spans="13:13">
+      <c r="M45" s="1" t="s">
+        <v>802</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AD4BEE2-D5EC-4736-9D22-FF1341A23CF9}">
+  <dimension ref="A1:M43"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="M43" sqref="M43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>841</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="M3" s="1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="2"/>
+      <c r="E4" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>840</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="M6" s="1" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="2"/>
+      <c r="E8" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="2"/>
+      <c r="E12" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="2"/>
+      <c r="E16" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="1" t="s">
+        <v>807</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>826</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="2"/>
+      <c r="I20" s="1" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="2"/>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="1" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" s="2"/>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" s="1" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="13:13">
+      <c r="M43" s="1" t="s">
+        <v>844</v>
       </c>
     </row>
   </sheetData>
@@ -8701,6 +9860,205 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA1A1B2E-8C1D-4327-AB04-F9E850DBBE43}">
+  <dimension ref="A1:E31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10:E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>845</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2"/>
+      <c r="E4" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2"/>
+      <c r="E8" s="1" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2"/>
+      <c r="E12" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="E13" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="1" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="1" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="2"/>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="2"/>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="1" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>